<commit_message>
Added related publication to promonitor OLR
</commit_message>
<xml_diff>
--- a/datamares/OLR/OLR_datamares_promonitor.xlsx
+++ b/datamares/OLR/OLR_datamares_promonitor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="665">
   <si>
     <t>text</t>
   </si>
@@ -2016,6 +2016,9 @@
   </si>
   <si>
     <t>Fish | Marine invertebrates | Underwater</t>
+  </si>
+  <si>
+    <t>Aburto-Oropeza O, et al (2014) A framework to assess the health of rocky reefs linking geomorphology, community assemblage, and fish biomass. Ecological Indicators 52:353-361. http://dx.doi.org/10.1016/j.ecolind.2014.12.006.</t>
   </si>
 </sst>
 </file>
@@ -3314,12 +3317,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG11"/>
+  <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R1" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,15 +3341,15 @@
     <col min="13" max="13" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="39.140625" style="24" customWidth="1"/>
-    <col min="17" max="17" width="39.140625" style="26" customWidth="1"/>
-    <col min="18" max="21" width="39.140625" style="24" customWidth="1"/>
-    <col min="22" max="23" width="42.85546875" style="3" customWidth="1"/>
-    <col min="24" max="24" width="47.85546875" style="3" customWidth="1"/>
-    <col min="25" max="25" width="49.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="33" width="35" customWidth="1"/>
+    <col min="17" max="18" width="39.140625" style="26" customWidth="1"/>
+    <col min="19" max="22" width="39.140625" style="24" customWidth="1"/>
+    <col min="23" max="24" width="42.85546875" style="3" customWidth="1"/>
+    <col min="25" max="25" width="47.85546875" style="3" customWidth="1"/>
+    <col min="26" max="26" width="49.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="34" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3398,26 +3401,26 @@
       <c r="Q1" s="25" t="s">
         <v>352</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="S1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>354</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>507</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>506</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="W1" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="X1" s="16" t="s">
         <v>455</v>
-      </c>
-      <c r="X1" s="16" t="s">
-        <v>483</v>
       </c>
       <c r="Y1" s="16" t="s">
         <v>483</v>
@@ -3446,8 +3449,11 @@
       <c r="AG1" s="16" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" s="18" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH1" s="16" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" s="18" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>621</v>
       </c>
@@ -3497,32 +3503,35 @@
         <v>657</v>
       </c>
       <c r="Q2" s="26"/>
-      <c r="R2" s="22" t="s">
+      <c r="R2" s="26" t="s">
+        <v>664</v>
+      </c>
+      <c r="S2" s="22" t="s">
         <v>627</v>
       </c>
-      <c r="S2" s="23" t="s">
+      <c r="T2" s="23" t="s">
         <v>652</v>
       </c>
-      <c r="T2" s="22" t="s">
+      <c r="U2" s="22" t="s">
         <v>655</v>
       </c>
-      <c r="U2" s="22" t="s">
+      <c r="V2" s="22" t="s">
         <v>633</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="W2" s="17" t="s">
         <v>662</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="X2" s="17" t="s">
         <v>653</v>
       </c>
-      <c r="X2" s="19" t="s">
+      <c r="Y2" s="19" t="s">
         <v>634</v>
       </c>
-      <c r="Y2" s="18" t="s">
+      <c r="Z2" s="18" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="18" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" s="18" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>656</v>
       </c>
@@ -3574,86 +3583,87 @@
       <c r="Q3" s="26" t="s">
         <v>658</v>
       </c>
-      <c r="R3" s="22" t="s">
+      <c r="R3" s="26"/>
+      <c r="S3" s="22" t="s">
         <v>641</v>
       </c>
-      <c r="S3" s="23" t="s">
+      <c r="T3" s="23" t="s">
         <v>642</v>
       </c>
-      <c r="T3" s="22" t="s">
+      <c r="U3" s="22" t="s">
         <v>655</v>
       </c>
-      <c r="U3" s="22" t="s">
+      <c r="V3" s="22" t="s">
         <v>643</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="W3" s="17" t="s">
         <v>663</v>
       </c>
-      <c r="W3" s="17" t="s">
+      <c r="X3" s="17" t="s">
         <v>661</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="Y3" s="18" t="s">
         <v>645</v>
       </c>
-      <c r="Y3" s="19" t="s">
+      <c r="Z3" s="19" t="s">
         <v>644</v>
       </c>
-      <c r="Z3" s="19" t="s">
+      <c r="AA3" s="19" t="s">
         <v>646</v>
       </c>
-      <c r="AA3" s="19" t="s">
+      <c r="AB3" s="19" t="s">
         <v>647</v>
       </c>
-      <c r="AB3" s="19" t="s">
+      <c r="AC3" s="19" t="s">
         <v>634</v>
       </c>
-      <c r="AC3" s="19" t="s">
+      <c r="AD3" s="19" t="s">
         <v>635</v>
       </c>
-      <c r="AD3" s="19" t="s">
+      <c r="AE3" s="19" t="s">
         <v>649</v>
       </c>
-      <c r="AE3" s="19" t="s">
+      <c r="AF3" s="19" t="s">
         <v>648</v>
       </c>
-      <c r="AF3" s="19" t="s">
+      <c r="AG3" s="19" t="s">
         <v>651</v>
       </c>
-      <c r="AG3" s="19" t="s">
+      <c r="AH3" s="19" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="T4" s="22"/>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U4" s="22"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="J5" s="17"/>
-      <c r="T5" s="22"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="U5" s="22"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
-      <c r="T6" s="22"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="U6" s="22"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="K7" s="17"/>
-      <c r="T7" s="22"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="U7" s="22"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="M8" s="20"/>
-      <c r="T8" s="22"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="U8" s="22"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="J9" s="17"/>
-      <c r="T9" s="22"/>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="U9" s="22"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="J10" s="17"/>
-      <c r="T10" s="22"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="U10" s="22"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="I11" s="17"/>
-      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10:B1048576 B1:B2 B4">
@@ -3836,19 +3846,19 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$13</xm:f>
           </x14:formula1>
-          <xm:sqref>V1:W1</xm:sqref>
+          <xm:sqref>W1:X1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>X1:AG1</xm:sqref>
+          <xm:sqref>Y1:AH1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$30</xm:f>
           </x14:formula1>
-          <xm:sqref>P1:U1</xm:sqref>
+          <xm:sqref>P1:V1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>

</xml_diff>

<commit_message>
Prepared promonitor OLR for test ingest
</commit_message>
<xml_diff>
--- a/datamares/OLR/OLR_datamares_promonitor.xlsx
+++ b/datamares/OLR/OLR_datamares_promonitor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="664">
   <si>
     <t>text</t>
   </si>
@@ -1934,9 +1934,6 @@
     <t>Indice de Salud @ http://dx.doi.org/10.13022/M35P4B</t>
   </si>
   <si>
-    <t>p_gc_promonitor.xlsx</t>
-  </si>
-  <si>
     <t>Monitoring Program of Gulf of California and Pacific coast (ProMonitor)</t>
   </si>
   <si>
@@ -2018,7 +2015,7 @@
     <t>Fish | Marine invertebrates | Underwater</t>
   </si>
   <si>
-    <t>Aburto-Oropeza O, et al (2014) A framework to assess the health of rocky reefs linking geomorphology, community assemblage, and fish biomass. Ecological Indicators 52:353-361. http://dx.doi.org/10.1016/j.ecolind.2014.12.006.</t>
+    <t>Aburto-Oropeza O, et al (2014) A framework to assess the health of rocky reefs linking geomorphology, community assemblage, and fish biomass. Ecological Indicators 52:353-361. http://dx.doi.org/10.1016/j.ecolind.2014.12.006</t>
   </si>
 </sst>
 </file>
@@ -3319,10 +3316,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R1" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3479,7 +3476,7 @@
         <v>626</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>624</v>
@@ -3500,29 +3497,29 @@
         <v>631</v>
       </c>
       <c r="P2" s="22" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="Q2" s="26"/>
       <c r="R2" s="26" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="S2" s="22" t="s">
         <v>627</v>
       </c>
       <c r="T2" s="23" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="U2" s="22" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="V2" s="22" t="s">
         <v>633</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="Y2" s="19" t="s">
         <v>634</v>
@@ -3533,20 +3530,14 @@
     </row>
     <row r="3" spans="1:34" s="18" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>485</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>636</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>473</v>
-      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="17" t="s">
         <v>358</v>
       </c>
@@ -3554,13 +3545,13 @@
         <v>433</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="K3" s="17" t="s">
         <v>622</v>
@@ -3569,50 +3560,50 @@
         <v>625</v>
       </c>
       <c r="M3" s="17" t="s">
+        <v>637</v>
+      </c>
+      <c r="N3" s="17" t="s">
         <v>638</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="O3" s="17" t="s">
         <v>639</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>640</v>
       </c>
       <c r="P3" s="22" t="s">
         <v>625</v>
       </c>
       <c r="Q3" s="26" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="R3" s="26"/>
       <c r="S3" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="T3" s="23" t="s">
         <v>641</v>
       </c>
-      <c r="T3" s="23" t="s">
+      <c r="U3" s="22" t="s">
+        <v>654</v>
+      </c>
+      <c r="V3" s="22" t="s">
         <v>642</v>
       </c>
-      <c r="U3" s="22" t="s">
-        <v>655</v>
-      </c>
-      <c r="V3" s="22" t="s">
+      <c r="W3" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="X3" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="Y3" s="18" t="s">
+        <v>644</v>
+      </c>
+      <c r="Z3" s="19" t="s">
         <v>643</v>
       </c>
-      <c r="W3" s="17" t="s">
-        <v>663</v>
-      </c>
-      <c r="X3" s="17" t="s">
-        <v>661</v>
-      </c>
-      <c r="Y3" s="18" t="s">
+      <c r="AA3" s="19" t="s">
         <v>645</v>
       </c>
-      <c r="Z3" s="19" t="s">
-        <v>644</v>
-      </c>
-      <c r="AA3" s="19" t="s">
+      <c r="AB3" s="19" t="s">
         <v>646</v>
-      </c>
-      <c r="AB3" s="19" t="s">
-        <v>647</v>
       </c>
       <c r="AC3" s="19" t="s">
         <v>634</v>
@@ -3621,16 +3612,16 @@
         <v>635</v>
       </c>
       <c r="AE3" s="19" t="s">
+        <v>648</v>
+      </c>
+      <c r="AF3" s="19" t="s">
+        <v>647</v>
+      </c>
+      <c r="AG3" s="19" t="s">
+        <v>650</v>
+      </c>
+      <c r="AH3" s="19" t="s">
         <v>649</v>
-      </c>
-      <c r="AF3" s="19" t="s">
-        <v>648</v>
-      </c>
-      <c r="AG3" s="19" t="s">
-        <v>651</v>
-      </c>
-      <c r="AH3" s="19" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">

</xml_diff>